<commit_message>
Carga de spinner: esta debe desaparecer antes cuando se muestre el modal de success
</commit_message>
<xml_diff>
--- a/Client/public/plantillaCall.xlsx
+++ b/Client/public/plantillaCall.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC1\Desktop\Nuevo\Manager_wsp\Manager_wsp\Client\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1832FFE-8EE1-4638-BB34-4FC4FBE8FC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F1F6D1-9B25-429E-A29D-CA4DD9BF87C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6915" yWindow="3255" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -432,12 +432,12 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,31 +447,33 @@
       <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3">
+        <v>932000076</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>